<commit_message>
nowe ui , poprawa logiki
</commit_message>
<xml_diff>
--- a/szablon.xlsx
+++ b/szablon.xlsx
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
-  <si>
-    <t xml:space="preserve">Imie i nazwisko pacjenta: </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">Imię i nazwisko pacjenta: </t>
   </si>
   <si>
     <t xml:space="preserve">Oddział</t>
@@ -49,10 +49,13 @@
     <t xml:space="preserve">Dożylna droga podania mieszaniny:  </t>
   </si>
   <si>
-    <t xml:space="preserve">Obwodowa</t>
+    <t xml:space="preserve">Obwodowa X</t>
   </si>
   <si>
     <t xml:space="preserve">Nr recepty:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centralna</t>
   </si>
   <si>
     <t xml:space="preserve">Czas podania:</t>
@@ -796,8 +799,8 @@
   </sheetPr>
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,7 +1020,9 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="13"/>
+      <c r="C12" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -1049,19 +1054,19 @@
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="14"/>
       <c r="F14" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1079,7 +1084,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1117,10 +1122,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -1152,7 +1157,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -1161,7 +1166,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
@@ -1172,10 +1177,10 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -1183,10 +1188,10 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1196,22 +1201,22 @@
       <c r="A22" s="18"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
@@ -1224,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
@@ -1243,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -1262,7 +1267,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -1281,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="22" t="n">
         <v>500</v>
@@ -1320,7 +1325,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="24"/>
@@ -1339,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="28" t="n">
@@ -1360,7 +1365,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="29" t="n">
@@ -1381,10 +1386,12 @@
         <v>9</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" s="23"/>
-      <c r="D31" s="29"/>
+      <c r="D31" s="29" t="n">
+        <v>10</v>
+      </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
@@ -1400,7 +1407,7 @@
         <v>10</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="23" t="n">
@@ -1421,7 +1428,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="28"/>
@@ -1440,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="23" t="n">
@@ -1461,7 +1468,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="28" t="n">
@@ -1482,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="28"/>
@@ -1501,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="23" t="n">
@@ -1522,7 +1529,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="28" t="n">
@@ -1543,7 +1550,7 @@
         <v>17</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
@@ -1562,7 +1569,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="28" t="n">
@@ -1583,7 +1590,7 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="28" t="n">
@@ -1604,7 +1611,7 @@
         <v>20</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="28" t="n">
@@ -1625,7 +1632,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="n">
@@ -1646,7 +1653,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="23"/>
@@ -1665,7 +1672,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="23"/>
@@ -1684,7 +1691,7 @@
         <v>24</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
@@ -1703,7 +1710,7 @@
         <v>25</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
@@ -1750,7 +1757,7 @@
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C50" s="38"/>
       <c r="D50" s="38"/>
@@ -1758,7 +1765,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
@@ -1785,7 +1792,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="39" t="str">
         <f aca="false">CONCATENATE(B66,C66)</f>
-        <v>1725ml</v>
+        <v>1735ml</v>
       </c>
       <c r="C52" s="39"/>
       <c r="D52" s="39"/>
@@ -1817,13 +1824,13 @@
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="3"/>
       <c r="F54" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -1851,13 +1858,13 @@
     <row r="56" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="3"/>
       <c r="F56" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -1870,14 +1877,14 @@
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="1" t="n">
         <f aca="false">SUM(D23:D44)</f>
-        <v>1725</v>
+        <v>1735</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="28">
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:E5"/>
     <mergeCell ref="G2:M9"/>
@@ -1899,7 +1906,6 @@
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
-    <mergeCell ref="D30:D31"/>
     <mergeCell ref="B50:E51"/>
     <mergeCell ref="H50:J52"/>
     <mergeCell ref="B52:E52"/>

</xml_diff>